<commit_message>
Just pushing the files please check the files i have pushed and tell me if any changes needed
</commit_message>
<xml_diff>
--- a/Reports and Deliverables/Initial Project Report/Revised Gantt Chart.xlsx
+++ b/Reports and Deliverables/Initial Project Report/Revised Gantt Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhavj\OneDrive\Desktop\Bhavjot UNI\Second Year (Level 5)\Data Science Project Lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhavj\DLP_CW\Reports and Deliverables\Initial Project Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0EE6A7-19AE-455A-B69A-8C0AD0445B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42D0013-6CD7-43EF-9F19-105818EEBD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{4FB197A3-E416-4451-B051-7D38F84165C7}"/>
   </bookViews>
@@ -803,7 +803,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>